<commit_message>
add total yield col. info
</commit_message>
<xml_diff>
--- a/data/master-qubit.xlsx
+++ b/data/master-qubit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DD3AB8-6EB9-B44A-BC30-73226499990B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5824FF85-444A-BA45-8574-E8E811CFEEB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="460" windowWidth="25480" windowHeight="14900" xr2:uid="{C961D9B2-DEF5-3E45-BFAA-11F0CD1F34D4}"/>
   </bookViews>
@@ -1878,7 +1878,7 @@
   <dimension ref="A1:S402"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="J301" sqref="J301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1978,6 +1978,13 @@
       <c r="K2" t="s">
         <v>332</v>
       </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
+      <c r="M2">
+        <f>(F2)*(L2-G2)</f>
+        <v>35.840000000000003</v>
+      </c>
       <c r="N2" t="s">
         <v>398</v>
       </c>
@@ -2019,6 +2026,13 @@
       <c r="K3" t="s">
         <v>332</v>
       </c>
+      <c r="L3">
+        <v>50</v>
+      </c>
+      <c r="M3" t="e">
+        <f>(F3)*(L3-G3)</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="N3" t="s">
         <v>398</v>
       </c>
@@ -2060,6 +2074,13 @@
       <c r="K4" t="s">
         <v>332</v>
       </c>
+      <c r="L4">
+        <v>50</v>
+      </c>
+      <c r="M4">
+        <f>(F4)*(L4-G4)</f>
+        <v>76.95</v>
+      </c>
       <c r="N4" t="s">
         <v>398</v>
       </c>
@@ -2101,6 +2122,13 @@
       <c r="K5" t="s">
         <v>332</v>
       </c>
+      <c r="L5">
+        <v>50</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M7" si="0">(F5)*(L5-G5)</f>
+        <v>0</v>
+      </c>
       <c r="N5" t="s">
         <v>398</v>
       </c>
@@ -2142,6 +2170,13 @@
       <c r="K6" t="s">
         <v>332</v>
       </c>
+      <c r="L6">
+        <v>50</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
       <c r="N6" t="s">
         <v>398</v>
       </c>
@@ -2183,6 +2218,13 @@
       <c r="K7" t="s">
         <v>332</v>
       </c>
+      <c r="L7">
+        <v>50</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N7" t="s">
         <v>398</v>
       </c>
@@ -2224,6 +2266,13 @@
       <c r="K8" t="s">
         <v>332</v>
       </c>
+      <c r="L8">
+        <v>50</v>
+      </c>
+      <c r="M8">
+        <f>(F8)*(L8-G8)</f>
+        <v>0</v>
+      </c>
       <c r="N8" t="s">
         <v>398</v>
       </c>
@@ -2265,6 +2314,13 @@
       <c r="K9" t="s">
         <v>332</v>
       </c>
+      <c r="L9">
+        <v>50</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ref="M9:M11" si="1">(F9)*(L9-G9)</f>
+        <v>81</v>
+      </c>
       <c r="N9" t="s">
         <v>398</v>
       </c>
@@ -2306,6 +2362,13 @@
       <c r="K10" t="s">
         <v>332</v>
       </c>
+      <c r="L10">
+        <v>50</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>52.199999999999996</v>
+      </c>
       <c r="N10" t="s">
         <v>398</v>
       </c>
@@ -2347,6 +2410,13 @@
       <c r="K11" t="s">
         <v>332</v>
       </c>
+      <c r="L11">
+        <v>50</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>232.20000000000002</v>
+      </c>
       <c r="N11" t="s">
         <v>398</v>
       </c>
@@ -8482,6 +8552,13 @@
       <c r="K170" t="s">
         <v>332</v>
       </c>
+      <c r="L170">
+        <v>14</v>
+      </c>
+      <c r="M170" t="e">
+        <f>(F170)*(L170-G170)</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="N170" t="s">
         <v>398</v>
       </c>
@@ -8523,6 +8600,13 @@
       <c r="K171" t="s">
         <v>332</v>
       </c>
+      <c r="L171">
+        <v>14</v>
+      </c>
+      <c r="M171">
+        <f t="shared" ref="M171:M209" si="2">(F171)*(L171-G171)</f>
+        <v>234</v>
+      </c>
       <c r="N171" t="s">
         <v>398</v>
       </c>
@@ -8564,6 +8648,13 @@
       <c r="K172" t="s">
         <v>332</v>
       </c>
+      <c r="L172">
+        <v>14</v>
+      </c>
+      <c r="M172" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N172" t="s">
         <v>398</v>
       </c>
@@ -8605,6 +8696,13 @@
       <c r="K173" t="s">
         <v>332</v>
       </c>
+      <c r="L173">
+        <v>14</v>
+      </c>
+      <c r="M173" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N173" t="s">
         <v>398</v>
       </c>
@@ -8646,6 +8744,13 @@
       <c r="K174" t="s">
         <v>332</v>
       </c>
+      <c r="L174">
+        <v>14</v>
+      </c>
+      <c r="M174">
+        <f t="shared" si="2"/>
+        <v>224.9</v>
+      </c>
       <c r="N174" t="s">
         <v>398</v>
       </c>
@@ -8687,6 +8792,13 @@
       <c r="K175" t="s">
         <v>332</v>
       </c>
+      <c r="L175">
+        <v>14</v>
+      </c>
+      <c r="M175">
+        <f t="shared" si="2"/>
+        <v>387.40000000000003</v>
+      </c>
       <c r="N175" t="s">
         <v>398</v>
       </c>
@@ -8728,6 +8840,13 @@
       <c r="K176" t="s">
         <v>332</v>
       </c>
+      <c r="L176">
+        <v>14</v>
+      </c>
+      <c r="M176" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N176" t="s">
         <v>398</v>
       </c>
@@ -8769,6 +8888,13 @@
       <c r="K177" t="s">
         <v>332</v>
       </c>
+      <c r="L177">
+        <v>14</v>
+      </c>
+      <c r="M177">
+        <f t="shared" si="2"/>
+        <v>68.64</v>
+      </c>
       <c r="N177" t="s">
         <v>398</v>
       </c>
@@ -8810,6 +8936,13 @@
       <c r="K178" t="s">
         <v>332</v>
       </c>
+      <c r="L178">
+        <v>14</v>
+      </c>
+      <c r="M178">
+        <f t="shared" si="2"/>
+        <v>108.94000000000001</v>
+      </c>
       <c r="N178" t="s">
         <v>398</v>
       </c>
@@ -8851,6 +8984,13 @@
       <c r="K179" t="s">
         <v>332</v>
       </c>
+      <c r="L179">
+        <v>14</v>
+      </c>
+      <c r="M179" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N179" t="s">
         <v>398</v>
       </c>
@@ -8892,6 +9032,13 @@
       <c r="K180" t="s">
         <v>332</v>
       </c>
+      <c r="L180">
+        <v>14</v>
+      </c>
+      <c r="M180">
+        <f t="shared" si="2"/>
+        <v>90.22</v>
+      </c>
       <c r="N180" t="s">
         <v>398</v>
       </c>
@@ -8933,6 +9080,13 @@
       <c r="K181" t="s">
         <v>332</v>
       </c>
+      <c r="L181">
+        <v>14</v>
+      </c>
+      <c r="M181">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
       <c r="N181" t="s">
         <v>398</v>
       </c>
@@ -8974,6 +9128,13 @@
       <c r="K182" t="s">
         <v>332</v>
       </c>
+      <c r="L182">
+        <v>14</v>
+      </c>
+      <c r="M182">
+        <f t="shared" si="2"/>
+        <v>94.64</v>
+      </c>
       <c r="N182" t="s">
         <v>398</v>
       </c>
@@ -9015,6 +9176,13 @@
       <c r="K183" t="s">
         <v>332</v>
       </c>
+      <c r="L183">
+        <v>14</v>
+      </c>
+      <c r="M183" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N183" t="s">
         <v>398</v>
       </c>
@@ -9056,6 +9224,13 @@
       <c r="K184" t="s">
         <v>332</v>
       </c>
+      <c r="L184">
+        <v>14</v>
+      </c>
+      <c r="M184" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N184" t="s">
         <v>398</v>
       </c>
@@ -9097,6 +9272,13 @@
       <c r="K185" t="s">
         <v>332</v>
       </c>
+      <c r="L185">
+        <v>14</v>
+      </c>
+      <c r="M185">
+        <f t="shared" si="2"/>
+        <v>93.600000000000009</v>
+      </c>
       <c r="N185" t="s">
         <v>398</v>
       </c>
@@ -9138,6 +9320,13 @@
       <c r="K186" t="s">
         <v>332</v>
       </c>
+      <c r="L186">
+        <v>14</v>
+      </c>
+      <c r="M186">
+        <f t="shared" si="2"/>
+        <v>206.70000000000002</v>
+      </c>
       <c r="N186" t="s">
         <v>398</v>
       </c>
@@ -9179,6 +9368,13 @@
       <c r="K187" t="s">
         <v>332</v>
       </c>
+      <c r="L187">
+        <v>14</v>
+      </c>
+      <c r="M187" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N187" t="s">
         <v>398</v>
       </c>
@@ -9220,6 +9416,13 @@
       <c r="K188" t="s">
         <v>332</v>
       </c>
+      <c r="L188">
+        <v>14</v>
+      </c>
+      <c r="M188" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N188" t="s">
         <v>398</v>
       </c>
@@ -9261,6 +9464,13 @@
       <c r="K189" t="s">
         <v>332</v>
       </c>
+      <c r="L189">
+        <v>14</v>
+      </c>
+      <c r="M189" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N189" t="s">
         <v>398</v>
       </c>
@@ -9302,6 +9512,13 @@
       <c r="K190" t="s">
         <v>332</v>
       </c>
+      <c r="L190">
+        <v>14</v>
+      </c>
+      <c r="M190" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N190" t="s">
         <v>398</v>
       </c>
@@ -9343,6 +9560,13 @@
       <c r="K191" t="s">
         <v>332</v>
       </c>
+      <c r="L191">
+        <v>14</v>
+      </c>
+      <c r="M191" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N191" t="s">
         <v>398</v>
       </c>
@@ -9384,6 +9608,13 @@
       <c r="K192" t="s">
         <v>332</v>
       </c>
+      <c r="L192">
+        <v>14</v>
+      </c>
+      <c r="M192">
+        <f t="shared" si="2"/>
+        <v>62.4</v>
+      </c>
       <c r="N192" t="s">
         <v>398</v>
       </c>
@@ -9425,6 +9656,13 @@
       <c r="K193" t="s">
         <v>332</v>
       </c>
+      <c r="L193">
+        <v>14</v>
+      </c>
+      <c r="M193" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N193" t="s">
         <v>398</v>
       </c>
@@ -9466,6 +9704,13 @@
       <c r="K194" t="s">
         <v>332</v>
       </c>
+      <c r="L194">
+        <v>14</v>
+      </c>
+      <c r="M194" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N194" t="s">
         <v>398</v>
       </c>
@@ -9507,6 +9752,13 @@
       <c r="K195" t="s">
         <v>332</v>
       </c>
+      <c r="L195">
+        <v>14</v>
+      </c>
+      <c r="M195">
+        <f t="shared" si="2"/>
+        <v>89.18</v>
+      </c>
       <c r="N195" t="s">
         <v>398</v>
       </c>
@@ -9548,6 +9800,13 @@
       <c r="K196" t="s">
         <v>332</v>
       </c>
+      <c r="L196">
+        <v>14</v>
+      </c>
+      <c r="M196" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N196" t="s">
         <v>398</v>
       </c>
@@ -9589,6 +9848,13 @@
       <c r="K197" t="s">
         <v>332</v>
       </c>
+      <c r="L197">
+        <v>14</v>
+      </c>
+      <c r="M197" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N197" t="s">
         <v>398</v>
       </c>
@@ -9630,6 +9896,13 @@
       <c r="K198" t="s">
         <v>332</v>
       </c>
+      <c r="L198">
+        <v>14</v>
+      </c>
+      <c r="M198">
+        <f t="shared" si="2"/>
+        <v>118.55999999999999</v>
+      </c>
       <c r="N198" t="s">
         <v>398</v>
       </c>
@@ -9671,6 +9944,13 @@
       <c r="K199" t="s">
         <v>332</v>
       </c>
+      <c r="L199">
+        <v>14</v>
+      </c>
+      <c r="M199">
+        <f t="shared" si="2"/>
+        <v>71.759999999999991</v>
+      </c>
       <c r="N199" t="s">
         <v>398</v>
       </c>
@@ -9712,6 +9992,13 @@
       <c r="K200" t="s">
         <v>332</v>
       </c>
+      <c r="L200">
+        <v>14</v>
+      </c>
+      <c r="M200">
+        <f t="shared" si="2"/>
+        <v>126.62</v>
+      </c>
       <c r="N200" t="s">
         <v>398</v>
       </c>
@@ -9753,6 +10040,13 @@
       <c r="K201" t="s">
         <v>332</v>
       </c>
+      <c r="L201">
+        <v>14</v>
+      </c>
+      <c r="M201" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N201" t="s">
         <v>398</v>
       </c>
@@ -9794,6 +10088,13 @@
       <c r="K202" t="s">
         <v>332</v>
       </c>
+      <c r="L202">
+        <v>14</v>
+      </c>
+      <c r="M202" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N202" t="s">
         <v>398</v>
       </c>
@@ -9835,6 +10136,13 @@
       <c r="K203" t="s">
         <v>332</v>
       </c>
+      <c r="L203">
+        <v>14</v>
+      </c>
+      <c r="M203" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N203" t="s">
         <v>398</v>
       </c>
@@ -9876,6 +10184,13 @@
       <c r="K204" t="s">
         <v>332</v>
       </c>
+      <c r="L204">
+        <v>14</v>
+      </c>
+      <c r="M204" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N204" t="s">
         <v>398</v>
       </c>
@@ -9917,6 +10232,13 @@
       <c r="K205" t="s">
         <v>332</v>
       </c>
+      <c r="L205">
+        <v>14</v>
+      </c>
+      <c r="M205" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N205" t="s">
         <v>398</v>
       </c>
@@ -9958,6 +10280,13 @@
       <c r="K206" t="s">
         <v>332</v>
       </c>
+      <c r="L206">
+        <v>14</v>
+      </c>
+      <c r="M206" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N206" t="s">
         <v>398</v>
       </c>
@@ -9999,6 +10328,13 @@
       <c r="K207" t="s">
         <v>332</v>
       </c>
+      <c r="L207">
+        <v>14</v>
+      </c>
+      <c r="M207" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N207" t="s">
         <v>398</v>
       </c>
@@ -10040,6 +10376,13 @@
       <c r="K208" t="s">
         <v>332</v>
       </c>
+      <c r="L208">
+        <v>14</v>
+      </c>
+      <c r="M208" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N208" t="s">
         <v>398</v>
       </c>
@@ -10081,6 +10424,13 @@
       <c r="K209" t="s">
         <v>332</v>
       </c>
+      <c r="L209">
+        <v>14</v>
+      </c>
+      <c r="M209" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N209" t="s">
         <v>398</v>
       </c>
@@ -11106,6 +11456,13 @@
       <c r="K234" t="s">
         <v>332</v>
       </c>
+      <c r="L234">
+        <v>14</v>
+      </c>
+      <c r="M234">
+        <f>(F234)*(L234-G234)</f>
+        <v>371.8</v>
+      </c>
       <c r="N234" t="s">
         <v>398</v>
       </c>
@@ -11147,6 +11504,13 @@
       <c r="K235" t="s">
         <v>332</v>
       </c>
+      <c r="L235">
+        <v>14</v>
+      </c>
+      <c r="M235">
+        <f t="shared" ref="M235:M245" si="3">(F235)*(L235-G235)</f>
+        <v>325</v>
+      </c>
       <c r="N235" t="s">
         <v>398</v>
       </c>
@@ -11234,6 +11598,13 @@
       <c r="K238" t="s">
         <v>332</v>
       </c>
+      <c r="L238">
+        <v>14</v>
+      </c>
+      <c r="M238">
+        <f t="shared" si="3"/>
+        <v>522.6</v>
+      </c>
       <c r="N238" t="s">
         <v>398</v>
       </c>
@@ -11275,6 +11646,13 @@
       <c r="K239" t="s">
         <v>332</v>
       </c>
+      <c r="L239">
+        <v>14</v>
+      </c>
+      <c r="M239">
+        <f t="shared" si="3"/>
+        <v>852.8</v>
+      </c>
       <c r="N239" t="s">
         <v>398</v>
       </c>
@@ -11316,6 +11694,13 @@
       <c r="K240" t="s">
         <v>332</v>
       </c>
+      <c r="L240">
+        <v>14</v>
+      </c>
+      <c r="M240">
+        <f t="shared" si="3"/>
+        <v>270.40000000000003</v>
+      </c>
       <c r="N240" t="s">
         <v>398</v>
       </c>
@@ -11357,6 +11742,13 @@
       <c r="K241" t="s">
         <v>332</v>
       </c>
+      <c r="L241">
+        <v>14</v>
+      </c>
+      <c r="M241">
+        <f t="shared" si="3"/>
+        <v>483.6</v>
+      </c>
       <c r="N241" t="s">
         <v>398</v>
       </c>
@@ -11398,6 +11790,13 @@
       <c r="K242" t="s">
         <v>332</v>
       </c>
+      <c r="L242">
+        <v>14</v>
+      </c>
+      <c r="M242">
+        <f t="shared" si="3"/>
+        <v>772.19999999999993</v>
+      </c>
       <c r="N242" t="s">
         <v>398</v>
       </c>
@@ -11439,6 +11838,13 @@
       <c r="K243" t="s">
         <v>332</v>
       </c>
+      <c r="L243">
+        <v>14</v>
+      </c>
+      <c r="M243">
+        <f t="shared" si="3"/>
+        <v>231.4</v>
+      </c>
       <c r="N243" t="s">
         <v>398</v>
       </c>
@@ -11480,6 +11886,13 @@
       <c r="K244" t="s">
         <v>332</v>
       </c>
+      <c r="L244">
+        <v>14</v>
+      </c>
+      <c r="M244" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N244" t="s">
         <v>398</v>
       </c>
@@ -11521,6 +11934,13 @@
       <c r="K245" t="s">
         <v>332</v>
       </c>
+      <c r="L245">
+        <v>14</v>
+      </c>
+      <c r="M245" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N245" t="s">
         <v>398</v>
       </c>
@@ -11784,6 +12204,9 @@
       <c r="F255" t="s">
         <v>4</v>
       </c>
+      <c r="G255">
+        <v>1</v>
+      </c>
       <c r="I255" t="s">
         <v>400</v>
       </c>
@@ -11793,6 +12216,13 @@
       <c r="K255" t="s">
         <v>332</v>
       </c>
+      <c r="L255">
+        <v>14</v>
+      </c>
+      <c r="M255" t="e">
+        <f>(F255)*(L255-G255)</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="N255" t="s">
         <v>399</v>
       </c>
@@ -11813,6 +12243,9 @@
       <c r="F256" t="s">
         <v>4</v>
       </c>
+      <c r="G256">
+        <v>1</v>
+      </c>
       <c r="I256" t="s">
         <v>401</v>
       </c>
@@ -11822,6 +12255,13 @@
       <c r="K256" t="s">
         <v>332</v>
       </c>
+      <c r="L256">
+        <v>14</v>
+      </c>
+      <c r="M256" t="e">
+        <f t="shared" ref="M256:M300" si="4">(F256)*(L256-G256)</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="N256" t="s">
         <v>399</v>
       </c>
@@ -11842,6 +12282,9 @@
       <c r="F257" t="s">
         <v>4</v>
       </c>
+      <c r="G257">
+        <v>1</v>
+      </c>
       <c r="I257" t="s">
         <v>402</v>
       </c>
@@ -11851,6 +12294,13 @@
       <c r="K257" t="s">
         <v>332</v>
       </c>
+      <c r="L257">
+        <v>14</v>
+      </c>
+      <c r="M257" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N257" t="s">
         <v>399</v>
       </c>
@@ -11871,6 +12321,9 @@
       <c r="F258" t="s">
         <v>4</v>
       </c>
+      <c r="G258">
+        <v>1</v>
+      </c>
       <c r="I258" t="s">
         <v>403</v>
       </c>
@@ -11880,6 +12333,13 @@
       <c r="K258" t="s">
         <v>332</v>
       </c>
+      <c r="L258">
+        <v>14</v>
+      </c>
+      <c r="M258" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N258" t="s">
         <v>399</v>
       </c>
@@ -11900,6 +12360,9 @@
       <c r="F259" t="s">
         <v>4</v>
       </c>
+      <c r="G259">
+        <v>1</v>
+      </c>
       <c r="I259" t="s">
         <v>405</v>
       </c>
@@ -11909,6 +12372,13 @@
       <c r="K259">
         <v>50</v>
       </c>
+      <c r="L259">
+        <v>14</v>
+      </c>
+      <c r="M259" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N259" t="s">
         <v>398</v>
       </c>
@@ -11929,6 +12399,9 @@
       <c r="F260" t="s">
         <v>4</v>
       </c>
+      <c r="G260">
+        <v>1</v>
+      </c>
       <c r="I260" t="s">
         <v>406</v>
       </c>
@@ -11938,6 +12411,13 @@
       <c r="K260">
         <v>50</v>
       </c>
+      <c r="L260">
+        <v>14</v>
+      </c>
+      <c r="M260" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N260" t="s">
         <v>398</v>
       </c>
@@ -11958,6 +12438,9 @@
       <c r="F261" t="s">
         <v>4</v>
       </c>
+      <c r="G261">
+        <v>1</v>
+      </c>
       <c r="I261" t="s">
         <v>407</v>
       </c>
@@ -11967,6 +12450,13 @@
       <c r="K261">
         <v>50</v>
       </c>
+      <c r="L261">
+        <v>14</v>
+      </c>
+      <c r="M261" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N261" t="s">
         <v>398</v>
       </c>
@@ -11984,6 +12474,9 @@
       <c r="F262">
         <v>7</v>
       </c>
+      <c r="G262">
+        <v>1</v>
+      </c>
       <c r="I262" t="s">
         <v>408</v>
       </c>
@@ -11992,6 +12485,13 @@
       </c>
       <c r="K262">
         <v>50</v>
+      </c>
+      <c r="L262">
+        <v>14</v>
+      </c>
+      <c r="M262">
+        <f t="shared" si="4"/>
+        <v>91</v>
       </c>
       <c r="N262" t="s">
         <v>398</v>
@@ -12019,6 +12519,9 @@
       <c r="F263" s="2">
         <v>14</v>
       </c>
+      <c r="G263">
+        <v>1</v>
+      </c>
       <c r="I263" t="s">
         <v>408</v>
       </c>
@@ -12027,6 +12530,13 @@
       </c>
       <c r="K263">
         <v>50</v>
+      </c>
+      <c r="L263">
+        <v>14</v>
+      </c>
+      <c r="M263">
+        <f t="shared" si="4"/>
+        <v>182</v>
       </c>
       <c r="N263" t="s">
         <v>398</v>
@@ -12057,6 +12567,9 @@
       <c r="F264" s="2">
         <v>4.5999999999999996</v>
       </c>
+      <c r="G264">
+        <v>1</v>
+      </c>
       <c r="I264" t="s">
         <v>408</v>
       </c>
@@ -12066,6 +12579,13 @@
       <c r="K264">
         <v>10</v>
       </c>
+      <c r="L264">
+        <v>14</v>
+      </c>
+      <c r="M264">
+        <f t="shared" si="4"/>
+        <v>59.8</v>
+      </c>
       <c r="N264" t="s">
         <v>398</v>
       </c>
@@ -12089,6 +12609,9 @@
       <c r="F265" t="s">
         <v>4</v>
       </c>
+      <c r="G265">
+        <v>1</v>
+      </c>
       <c r="I265">
         <v>135</v>
       </c>
@@ -12098,6 +12621,13 @@
       <c r="K265">
         <v>15</v>
       </c>
+      <c r="L265">
+        <v>14</v>
+      </c>
+      <c r="M265" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N265" t="s">
         <v>398</v>
       </c>
@@ -12118,6 +12648,9 @@
       <c r="F266" t="s">
         <v>4</v>
       </c>
+      <c r="G266">
+        <v>1</v>
+      </c>
       <c r="I266">
         <v>31</v>
       </c>
@@ -12127,6 +12660,13 @@
       <c r="K266">
         <v>15</v>
       </c>
+      <c r="L266">
+        <v>14</v>
+      </c>
+      <c r="M266" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N266" t="s">
         <v>398</v>
       </c>
@@ -12147,6 +12687,9 @@
       <c r="F267" t="s">
         <v>4</v>
       </c>
+      <c r="G267">
+        <v>1</v>
+      </c>
       <c r="I267">
         <v>90</v>
       </c>
@@ -12156,6 +12699,13 @@
       <c r="K267">
         <v>15</v>
       </c>
+      <c r="L267">
+        <v>14</v>
+      </c>
+      <c r="M267" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N267" t="s">
         <v>398</v>
       </c>
@@ -12176,6 +12726,9 @@
       <c r="F268" t="s">
         <v>4</v>
       </c>
+      <c r="G268">
+        <v>1</v>
+      </c>
       <c r="I268">
         <v>142</v>
       </c>
@@ -12185,6 +12738,13 @@
       <c r="K268">
         <v>15</v>
       </c>
+      <c r="L268">
+        <v>14</v>
+      </c>
+      <c r="M268" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N268" t="s">
         <v>398</v>
       </c>
@@ -12205,6 +12765,9 @@
       <c r="F269" t="s">
         <v>4</v>
       </c>
+      <c r="G269">
+        <v>1</v>
+      </c>
       <c r="I269">
         <v>317</v>
       </c>
@@ -12214,6 +12777,13 @@
       <c r="K269">
         <v>15</v>
       </c>
+      <c r="L269">
+        <v>14</v>
+      </c>
+      <c r="M269" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N269" t="s">
         <v>398</v>
       </c>
@@ -12234,6 +12804,9 @@
       <c r="F270" t="s">
         <v>4</v>
       </c>
+      <c r="G270">
+        <v>1</v>
+      </c>
       <c r="I270">
         <v>342</v>
       </c>
@@ -12243,6 +12816,13 @@
       <c r="K270">
         <v>15</v>
       </c>
+      <c r="L270">
+        <v>14</v>
+      </c>
+      <c r="M270" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N270" t="s">
         <v>398</v>
       </c>
@@ -12263,6 +12843,9 @@
       <c r="F271" t="s">
         <v>4</v>
       </c>
+      <c r="G271">
+        <v>1</v>
+      </c>
       <c r="I271">
         <v>352</v>
       </c>
@@ -12272,6 +12855,13 @@
       <c r="K271">
         <v>15</v>
       </c>
+      <c r="L271">
+        <v>14</v>
+      </c>
+      <c r="M271" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N271" t="s">
         <v>398</v>
       </c>
@@ -12292,6 +12882,9 @@
       <c r="F272" t="s">
         <v>4</v>
       </c>
+      <c r="G272">
+        <v>1</v>
+      </c>
       <c r="I272">
         <v>326</v>
       </c>
@@ -12301,6 +12894,13 @@
       <c r="K272">
         <v>15</v>
       </c>
+      <c r="L272">
+        <v>14</v>
+      </c>
+      <c r="M272" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N272" t="s">
         <v>398</v>
       </c>
@@ -12321,6 +12921,9 @@
       <c r="F273" t="s">
         <v>4</v>
       </c>
+      <c r="G273">
+        <v>1</v>
+      </c>
       <c r="I273">
         <v>242</v>
       </c>
@@ -12330,6 +12933,13 @@
       <c r="K273">
         <v>15</v>
       </c>
+      <c r="L273">
+        <v>14</v>
+      </c>
+      <c r="M273" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N273" t="s">
         <v>398</v>
       </c>
@@ -12350,6 +12960,9 @@
       <c r="F274" t="s">
         <v>4</v>
       </c>
+      <c r="G274">
+        <v>1</v>
+      </c>
       <c r="I274">
         <v>236</v>
       </c>
@@ -12359,6 +12972,13 @@
       <c r="K274">
         <v>15</v>
       </c>
+      <c r="L274">
+        <v>14</v>
+      </c>
+      <c r="M274" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N274" t="s">
         <v>398</v>
       </c>
@@ -12379,6 +12999,9 @@
       <c r="F275" t="s">
         <v>4</v>
       </c>
+      <c r="G275">
+        <v>1</v>
+      </c>
       <c r="I275">
         <v>234</v>
       </c>
@@ -12388,6 +13011,13 @@
       <c r="K275">
         <v>15</v>
       </c>
+      <c r="L275">
+        <v>14</v>
+      </c>
+      <c r="M275" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N275" t="s">
         <v>398</v>
       </c>
@@ -12408,6 +13038,9 @@
       <c r="F276" t="s">
         <v>4</v>
       </c>
+      <c r="G276">
+        <v>1</v>
+      </c>
       <c r="I276">
         <v>212</v>
       </c>
@@ -12417,6 +13050,13 @@
       <c r="K276">
         <v>15</v>
       </c>
+      <c r="L276">
+        <v>14</v>
+      </c>
+      <c r="M276" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N276" t="s">
         <v>398</v>
       </c>
@@ -12437,6 +13077,9 @@
       <c r="F277" t="s">
         <v>4</v>
       </c>
+      <c r="G277">
+        <v>1</v>
+      </c>
       <c r="I277">
         <v>285</v>
       </c>
@@ -12446,6 +13089,13 @@
       <c r="K277">
         <v>15</v>
       </c>
+      <c r="L277">
+        <v>14</v>
+      </c>
+      <c r="M277" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N277" t="s">
         <v>398</v>
       </c>
@@ -12466,6 +13116,9 @@
       <c r="F278" t="s">
         <v>4</v>
       </c>
+      <c r="G278">
+        <v>1</v>
+      </c>
       <c r="I278">
         <v>266</v>
       </c>
@@ -12475,6 +13128,13 @@
       <c r="K278">
         <v>15</v>
       </c>
+      <c r="L278">
+        <v>14</v>
+      </c>
+      <c r="M278" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N278" t="s">
         <v>398</v>
       </c>
@@ -12495,6 +13155,9 @@
       <c r="F279" t="s">
         <v>4</v>
       </c>
+      <c r="G279">
+        <v>1</v>
+      </c>
       <c r="I279">
         <v>271</v>
       </c>
@@ -12504,6 +13167,13 @@
       <c r="K279">
         <v>15</v>
       </c>
+      <c r="L279">
+        <v>14</v>
+      </c>
+      <c r="M279" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N279" t="s">
         <v>398</v>
       </c>
@@ -12524,6 +13194,9 @@
       <c r="F280" t="s">
         <v>4</v>
       </c>
+      <c r="G280">
+        <v>1</v>
+      </c>
       <c r="I280">
         <v>291</v>
       </c>
@@ -12533,6 +13206,13 @@
       <c r="K280">
         <v>15</v>
       </c>
+      <c r="L280">
+        <v>14</v>
+      </c>
+      <c r="M280" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N280" t="s">
         <v>398</v>
       </c>
@@ -12553,6 +13233,9 @@
       <c r="F281" t="s">
         <v>4</v>
       </c>
+      <c r="G281">
+        <v>1</v>
+      </c>
       <c r="I281">
         <v>499</v>
       </c>
@@ -12562,6 +13245,13 @@
       <c r="K281">
         <v>15</v>
       </c>
+      <c r="L281">
+        <v>14</v>
+      </c>
+      <c r="M281" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N281" t="s">
         <v>398</v>
       </c>
@@ -12582,6 +13272,9 @@
       <c r="F282" t="s">
         <v>4</v>
       </c>
+      <c r="G282">
+        <v>1</v>
+      </c>
       <c r="I282">
         <v>506</v>
       </c>
@@ -12591,6 +13284,13 @@
       <c r="K282">
         <v>15</v>
       </c>
+      <c r="L282">
+        <v>14</v>
+      </c>
+      <c r="M282" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N282" t="s">
         <v>398</v>
       </c>
@@ -12611,6 +13311,9 @@
       <c r="F283" t="s">
         <v>4</v>
       </c>
+      <c r="G283">
+        <v>1</v>
+      </c>
       <c r="I283">
         <v>468</v>
       </c>
@@ -12620,6 +13323,13 @@
       <c r="K283">
         <v>15</v>
       </c>
+      <c r="L283">
+        <v>14</v>
+      </c>
+      <c r="M283" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N283" t="s">
         <v>398</v>
       </c>
@@ -12640,6 +13350,9 @@
       <c r="F284" t="s">
         <v>4</v>
       </c>
+      <c r="G284">
+        <v>1</v>
+      </c>
       <c r="I284">
         <v>503</v>
       </c>
@@ -12649,6 +13362,13 @@
       <c r="K284">
         <v>15</v>
       </c>
+      <c r="L284">
+        <v>14</v>
+      </c>
+      <c r="M284" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N284" t="s">
         <v>398</v>
       </c>
@@ -12669,6 +13389,9 @@
       <c r="F285" t="s">
         <v>4</v>
       </c>
+      <c r="G285">
+        <v>1</v>
+      </c>
       <c r="I285">
         <v>458</v>
       </c>
@@ -12678,6 +13401,13 @@
       <c r="K285">
         <v>15</v>
       </c>
+      <c r="L285">
+        <v>14</v>
+      </c>
+      <c r="M285" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N285" t="s">
         <v>398</v>
       </c>
@@ -12698,6 +13428,9 @@
       <c r="F286" t="s">
         <v>4</v>
       </c>
+      <c r="G286">
+        <v>1</v>
+      </c>
       <c r="I286">
         <v>419</v>
       </c>
@@ -12707,6 +13440,13 @@
       <c r="K286">
         <v>15</v>
       </c>
+      <c r="L286">
+        <v>14</v>
+      </c>
+      <c r="M286" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N286" t="s">
         <v>398</v>
       </c>
@@ -12727,6 +13467,9 @@
       <c r="F287" t="s">
         <v>4</v>
       </c>
+      <c r="G287">
+        <v>1</v>
+      </c>
       <c r="I287">
         <v>438</v>
       </c>
@@ -12736,6 +13479,13 @@
       <c r="K287">
         <v>15</v>
       </c>
+      <c r="L287">
+        <v>14</v>
+      </c>
+      <c r="M287" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N287" t="s">
         <v>398</v>
       </c>
@@ -12756,6 +13506,9 @@
       <c r="F288" t="s">
         <v>4</v>
       </c>
+      <c r="G288">
+        <v>1</v>
+      </c>
       <c r="I288">
         <v>455</v>
       </c>
@@ -12764,6 +13517,13 @@
       </c>
       <c r="K288">
         <v>15</v>
+      </c>
+      <c r="L288">
+        <v>14</v>
+      </c>
+      <c r="M288" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N288" t="s">
         <v>398</v>
@@ -12806,8 +13566,13 @@
       <c r="K289" s="4">
         <v>15</v>
       </c>
-      <c r="L289" s="4"/>
-      <c r="M289" s="4"/>
+      <c r="L289">
+        <v>14</v>
+      </c>
+      <c r="M289" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N289" t="s">
         <v>398</v>
       </c>
@@ -12851,8 +13616,13 @@
       <c r="K290" s="4">
         <v>15</v>
       </c>
-      <c r="L290" s="4"/>
-      <c r="M290" s="4"/>
+      <c r="L290">
+        <v>14</v>
+      </c>
+      <c r="M290" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N290" t="s">
         <v>398</v>
       </c>
@@ -12896,8 +13666,13 @@
       <c r="K291" s="4">
         <v>15</v>
       </c>
-      <c r="L291" s="4"/>
-      <c r="M291" s="4"/>
+      <c r="L291">
+        <v>14</v>
+      </c>
+      <c r="M291" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N291" t="s">
         <v>398</v>
       </c>
@@ -12941,8 +13716,13 @@
       <c r="K292" s="4">
         <v>15</v>
       </c>
-      <c r="L292" s="4"/>
-      <c r="M292" s="4"/>
+      <c r="L292">
+        <v>14</v>
+      </c>
+      <c r="M292" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N292" t="s">
         <v>398</v>
       </c>
@@ -12986,8 +13766,13 @@
       <c r="K293" s="4">
         <v>15</v>
       </c>
-      <c r="L293" s="4"/>
-      <c r="M293" s="4"/>
+      <c r="L293">
+        <v>14</v>
+      </c>
+      <c r="M293" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N293" t="s">
         <v>398</v>
       </c>
@@ -13031,8 +13816,13 @@
       <c r="K294" s="4">
         <v>15</v>
       </c>
-      <c r="L294" s="4"/>
-      <c r="M294" s="4"/>
+      <c r="L294">
+        <v>14</v>
+      </c>
+      <c r="M294" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N294" t="s">
         <v>398</v>
       </c>
@@ -13076,8 +13866,13 @@
       <c r="K295" s="4">
         <v>15</v>
       </c>
-      <c r="L295" s="4"/>
-      <c r="M295" s="4"/>
+      <c r="L295">
+        <v>14</v>
+      </c>
+      <c r="M295" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N295" t="s">
         <v>398</v>
       </c>
@@ -13121,8 +13916,13 @@
       <c r="K296" s="4">
         <v>15</v>
       </c>
-      <c r="L296" s="4"/>
-      <c r="M296" s="4"/>
+      <c r="L296">
+        <v>14</v>
+      </c>
+      <c r="M296" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N296" t="s">
         <v>398</v>
       </c>
@@ -13166,8 +13966,13 @@
       <c r="K297" s="4">
         <v>15</v>
       </c>
-      <c r="L297" s="4"/>
-      <c r="M297" s="4"/>
+      <c r="L297">
+        <v>14</v>
+      </c>
+      <c r="M297" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N297" t="s">
         <v>398</v>
       </c>
@@ -13211,8 +14016,13 @@
       <c r="K298" s="4">
         <v>15</v>
       </c>
-      <c r="L298" s="4"/>
-      <c r="M298" s="4"/>
+      <c r="L298">
+        <v>14</v>
+      </c>
+      <c r="M298" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N298" t="s">
         <v>398</v>
       </c>
@@ -13256,8 +14066,13 @@
       <c r="K299" s="4">
         <v>15</v>
       </c>
-      <c r="L299" s="4"/>
-      <c r="M299" s="4"/>
+      <c r="L299">
+        <v>14</v>
+      </c>
+      <c r="M299" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N299" t="s">
         <v>398</v>
       </c>
@@ -13301,8 +14116,13 @@
       <c r="K300" s="4">
         <v>15</v>
       </c>
-      <c r="L300" s="4"/>
-      <c r="M300" s="4"/>
+      <c r="L300">
+        <v>14</v>
+      </c>
+      <c r="M300">
+        <f t="shared" si="4"/>
+        <v>59.8</v>
+      </c>
       <c r="N300" t="s">
         <v>398</v>
       </c>
@@ -14550,7 +15370,7 @@
         <v>15</v>
       </c>
       <c r="M338" s="4">
-        <f t="shared" ref="M338:M401" si="0">(F338)*(L338-G338)</f>
+        <f t="shared" ref="M338:M401" si="5">(F338)*(L338-G338)</f>
         <v>57.98</v>
       </c>
       <c r="N338" t="s">
@@ -14598,7 +15418,7 @@
         <v>15</v>
       </c>
       <c r="M339" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>265.2</v>
       </c>
       <c r="N339" t="s">
@@ -14646,7 +15466,7 @@
         <v>15</v>
       </c>
       <c r="M340" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>273</v>
       </c>
       <c r="N340" t="s">
@@ -14694,7 +15514,7 @@
         <v>15</v>
       </c>
       <c r="M341" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>427.7</v>
       </c>
       <c r="N341" t="s">
@@ -14742,7 +15562,7 @@
         <v>15</v>
       </c>
       <c r="M342" s="4" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N342" t="s">
@@ -14790,7 +15610,7 @@
         <v>15</v>
       </c>
       <c r="M343" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>451.1</v>
       </c>
       <c r="N343" t="s">
@@ -14838,7 +15658,7 @@
         <v>15</v>
       </c>
       <c r="M344" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>172.9</v>
       </c>
       <c r="N344" t="s">
@@ -14886,7 +15706,7 @@
         <v>15</v>
       </c>
       <c r="M345" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>378.3</v>
       </c>
       <c r="N345" t="s">
@@ -14934,7 +15754,7 @@
         <v>15</v>
       </c>
       <c r="M346" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>553.80000000000007</v>
       </c>
       <c r="N346" t="s">
@@ -14982,7 +15802,7 @@
         <v>15</v>
       </c>
       <c r="M347" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>495.3</v>
       </c>
       <c r="N347" t="s">
@@ -15030,7 +15850,7 @@
         <v>15</v>
       </c>
       <c r="M348" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>345.8</v>
       </c>
       <c r="N348" t="s">
@@ -15078,7 +15898,7 @@
         <v>15</v>
       </c>
       <c r="M349" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>663</v>
       </c>
       <c r="N349" t="s">
@@ -15126,7 +15946,7 @@
         <v>15</v>
       </c>
       <c r="M350" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>231.4</v>
       </c>
       <c r="N350" t="s">
@@ -15174,7 +15994,7 @@
         <v>15</v>
       </c>
       <c r="M351" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>936</v>
       </c>
       <c r="N351" t="s">
@@ -15222,7 +16042,7 @@
         <v>15</v>
       </c>
       <c r="M352" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>217.1</v>
       </c>
       <c r="N352" t="s">
@@ -15270,7 +16090,7 @@
         <v>15</v>
       </c>
       <c r="M353" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>590.19999999999993</v>
       </c>
       <c r="N353" t="s">
@@ -15318,7 +16138,7 @@
         <v>15</v>
       </c>
       <c r="M354" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>146.9</v>
       </c>
       <c r="N354" t="s">
@@ -15366,7 +16186,7 @@
         <v>15</v>
       </c>
       <c r="M355" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>198.9</v>
       </c>
       <c r="N355" t="s">
@@ -15414,7 +16234,7 @@
         <v>15</v>
       </c>
       <c r="M356" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>261.3</v>
       </c>
       <c r="N356" t="s">
@@ -15462,7 +16282,7 @@
         <v>15</v>
       </c>
       <c r="M357" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>319.8</v>
       </c>
       <c r="N357" t="s">
@@ -15510,7 +16330,7 @@
         <v>15</v>
       </c>
       <c r="M358" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>219.7</v>
       </c>
       <c r="N358" t="s">
@@ -15558,7 +16378,7 @@
         <v>15</v>
       </c>
       <c r="M359" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>258.7</v>
       </c>
       <c r="N359" t="s">
@@ -15606,7 +16426,7 @@
         <v>15</v>
       </c>
       <c r="M360" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>250.9</v>
       </c>
       <c r="N360" t="s">
@@ -15654,7 +16474,7 @@
         <v>15</v>
       </c>
       <c r="M361" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>397.8</v>
       </c>
       <c r="N361" t="s">
@@ -15702,7 +16522,7 @@
         <v>15</v>
       </c>
       <c r="M362" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>178.1</v>
       </c>
       <c r="N362" t="s">
@@ -15750,7 +16570,7 @@
         <v>15</v>
       </c>
       <c r="M363" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>310.7</v>
       </c>
       <c r="N363" t="s">
@@ -15798,7 +16618,7 @@
         <v>15</v>
       </c>
       <c r="M364" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>215.8</v>
       </c>
       <c r="N364" t="s">
@@ -15846,7 +16666,7 @@
         <v>15</v>
       </c>
       <c r="M365" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>232.7</v>
       </c>
       <c r="N365" t="s">
@@ -15894,7 +16714,7 @@
         <v>15</v>
       </c>
       <c r="M366" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>322.40000000000003</v>
       </c>
       <c r="N366" t="s">
@@ -15942,7 +16762,7 @@
         <v>15</v>
       </c>
       <c r="M367" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>98.02</v>
       </c>
       <c r="N367" t="s">
@@ -15990,7 +16810,7 @@
         <v>15</v>
       </c>
       <c r="M368" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>143</v>
       </c>
       <c r="N368" t="s">
@@ -16038,7 +16858,7 @@
         <v>15</v>
       </c>
       <c r="M369" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>284.7</v>
       </c>
       <c r="N369" t="s">
@@ -16086,7 +16906,7 @@
         <v>15</v>
       </c>
       <c r="M370" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>208</v>
       </c>
       <c r="N370" t="s">
@@ -16134,7 +16954,7 @@
         <v>15</v>
       </c>
       <c r="M371" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>202.79999999999998</v>
       </c>
       <c r="N371" t="s">
@@ -16182,7 +17002,7 @@
         <v>15</v>
       </c>
       <c r="M372" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>248.3</v>
       </c>
       <c r="N372" t="s">
@@ -16230,7 +17050,7 @@
         <v>15</v>
       </c>
       <c r="M373" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>244.4</v>
       </c>
       <c r="N373" t="s">
@@ -16278,7 +17098,7 @@
         <v>15</v>
       </c>
       <c r="M374" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>265.2</v>
       </c>
       <c r="N374" t="s">
@@ -16326,7 +17146,7 @@
         <v>15</v>
       </c>
       <c r="M375" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>176.79999999999998</v>
       </c>
       <c r="N375" t="s">
@@ -16374,7 +17194,7 @@
         <v>15</v>
       </c>
       <c r="M376" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>276.90000000000003</v>
       </c>
       <c r="N376" t="s">
@@ -16422,7 +17242,7 @@
         <v>15</v>
       </c>
       <c r="M377" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>274.3</v>
       </c>
       <c r="N377" t="s">
@@ -16470,7 +17290,7 @@
         <v>15</v>
       </c>
       <c r="M378" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>315.90000000000003</v>
       </c>
       <c r="N378" t="s">
@@ -16518,7 +17338,7 @@
         <v>15</v>
       </c>
       <c r="M379" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>409.5</v>
       </c>
       <c r="N379" t="s">
@@ -16566,7 +17386,7 @@
         <v>15</v>
       </c>
       <c r="M380" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>68.509999999999991</v>
       </c>
       <c r="N380" t="s">
@@ -16614,7 +17434,7 @@
         <v>15</v>
       </c>
       <c r="M381" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>133.9</v>
       </c>
       <c r="N381" t="s">
@@ -16662,7 +17482,7 @@
         <v>15</v>
       </c>
       <c r="M382" s="4" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N382" t="s">
@@ -16710,7 +17530,7 @@
         <v>15</v>
       </c>
       <c r="M383" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>158.6</v>
       </c>
       <c r="N383" t="s">
@@ -16758,7 +17578,7 @@
         <v>15</v>
       </c>
       <c r="M384" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>146.9</v>
       </c>
       <c r="N384" t="s">
@@ -16806,7 +17626,7 @@
         <v>15</v>
       </c>
       <c r="M385" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>82.94</v>
       </c>
       <c r="N385" t="s">
@@ -16854,7 +17674,7 @@
         <v>15</v>
       </c>
       <c r="M386" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>159.9</v>
       </c>
       <c r="N386" t="s">
@@ -16902,7 +17722,7 @@
         <v>15</v>
       </c>
       <c r="M387" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>388.7</v>
       </c>
       <c r="N387" t="s">
@@ -16950,7 +17770,7 @@
         <v>15</v>
       </c>
       <c r="M388" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>347.09999999999997</v>
       </c>
       <c r="N388" t="s">
@@ -16998,7 +17818,7 @@
         <v>15</v>
       </c>
       <c r="M389" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>280.8</v>
       </c>
       <c r="N389" t="s">
@@ -17046,7 +17866,7 @@
         <v>15</v>
       </c>
       <c r="M390" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>257.40000000000003</v>
       </c>
       <c r="N390" t="s">
@@ -17094,7 +17914,7 @@
         <v>15</v>
       </c>
       <c r="M391" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>132.6</v>
       </c>
       <c r="N391" t="s">
@@ -17142,7 +17962,7 @@
         <v>15</v>
       </c>
       <c r="M392" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>130</v>
       </c>
       <c r="N392" t="s">
@@ -17190,7 +18010,7 @@
         <v>15</v>
       </c>
       <c r="M393" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>258.7</v>
       </c>
       <c r="N393" t="s">
@@ -17238,7 +18058,7 @@
         <v>15</v>
       </c>
       <c r="M394" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>128.83000000000001</v>
       </c>
       <c r="N394" t="s">
@@ -17286,7 +18106,7 @@
         <v>15</v>
       </c>
       <c r="M395" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>257.40000000000003</v>
       </c>
       <c r="N395" t="s">
@@ -17334,7 +18154,7 @@
         <v>15</v>
       </c>
       <c r="M396" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>232.7</v>
       </c>
       <c r="N396" t="s">
@@ -17382,7 +18202,7 @@
         <v>15</v>
       </c>
       <c r="M397" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>309.40000000000003</v>
       </c>
       <c r="N397" t="s">
@@ -17430,7 +18250,7 @@
         <v>15</v>
       </c>
       <c r="M398" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>98.93</v>
       </c>
       <c r="N398" t="s">
@@ -17478,7 +18298,7 @@
         <v>15</v>
       </c>
       <c r="M399" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>304.2</v>
       </c>
       <c r="N399" t="s">
@@ -17526,7 +18346,7 @@
         <v>15</v>
       </c>
       <c r="M400" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>52.259999999999991</v>
       </c>
       <c r="N400" t="s">
@@ -17574,7 +18394,7 @@
         <v>15</v>
       </c>
       <c r="M401" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>253.5</v>
       </c>
       <c r="N401" t="s">
@@ -17622,7 +18442,7 @@
         <v>15</v>
       </c>
       <c r="M402" s="4">
-        <f t="shared" ref="M402" si="1">(F402)*(L402-G402)</f>
+        <f t="shared" ref="M402" si="6">(F402)*(L402-G402)</f>
         <v>171.6</v>
       </c>
       <c r="N402" t="s">

</xml_diff>

<commit_message>
add more - in progress
</commit_message>
<xml_diff>
--- a/data/master-qubit.xlsx
+++ b/data/master-qubit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5824FF85-444A-BA45-8574-E8E811CFEEB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187F310B-0046-C640-AAF1-AF736FACD731}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="460" windowWidth="25480" windowHeight="14900" xr2:uid="{C961D9B2-DEF5-3E45-BFAA-11F0CD1F34D4}"/>
   </bookViews>
@@ -1877,7 +1877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EE0E31-7CFF-2843-B4D6-D974DF19D232}">
   <dimension ref="A1:S402"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A378" workbookViewId="0">
       <selection activeCell="J301" sqref="J301"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add library and sequence info to spreadsheet
</commit_message>
<xml_diff>
--- a/data/master-qubit.xlsx
+++ b/data/master-qubit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC56571B-D01C-A24E-959D-95D0446D4957}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD49087-44B1-2F44-8814-A6E0D7A85C1A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="460" windowWidth="25560" windowHeight="14900" xr2:uid="{C961D9B2-DEF5-3E45-BFAA-11F0CD1F34D4}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2930" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3088" uniqueCount="502">
   <si>
     <t>tube_number</t>
   </si>
@@ -1529,6 +1529,15 @@
   </si>
   <si>
     <t>transcriptome_ID</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>pooled transcriptome - combined cold and ambient, infected and uninfected Day 26 (https://grace-ac.github.io/Pooled-sample-handed-toNWGC/)</t>
+  </si>
+  <si>
+    <t>https://robertslab.github.io/sams-notebook/2019/05/21/Sample-Submission-Tanner-Crab-Infected-vs-Uninfected-RNAseq.html</t>
   </si>
 </sst>
 </file>
@@ -1921,8 +1930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EE0E31-7CFF-2843-B4D6-D974DF19D232}">
   <dimension ref="A1:U402"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="I374" workbookViewId="0">
+      <selection activeCell="P393" sqref="P393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1936,7 +1945,8 @@
     <col min="8" max="8" width="13.1640625" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="16" width="14.5" customWidth="1"/>
+    <col min="11" max="15" width="14.5" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" customWidth="1"/>
     <col min="17" max="17" width="27" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9975,6 +9985,15 @@
       <c r="N171" t="s">
         <v>397</v>
       </c>
+      <c r="O171" t="s">
+        <v>499</v>
+      </c>
+      <c r="P171">
+        <v>1</v>
+      </c>
+      <c r="Q171" t="s">
+        <v>500</v>
+      </c>
       <c r="R171" t="s">
         <v>353</v>
       </c>
@@ -10119,6 +10138,15 @@
       <c r="N174" t="s">
         <v>397</v>
       </c>
+      <c r="O174" t="s">
+        <v>499</v>
+      </c>
+      <c r="P174">
+        <v>1</v>
+      </c>
+      <c r="Q174" t="s">
+        <v>500</v>
+      </c>
       <c r="R174" t="s">
         <v>353</v>
       </c>
@@ -10167,6 +10195,15 @@
       <c r="N175" t="s">
         <v>397</v>
       </c>
+      <c r="O175" t="s">
+        <v>499</v>
+      </c>
+      <c r="P175">
+        <v>1</v>
+      </c>
+      <c r="Q175" t="s">
+        <v>500</v>
+      </c>
       <c r="R175" t="s">
         <v>353</v>
       </c>
@@ -10263,6 +10300,15 @@
       <c r="N177" t="s">
         <v>397</v>
       </c>
+      <c r="O177" t="s">
+        <v>499</v>
+      </c>
+      <c r="P177">
+        <v>1</v>
+      </c>
+      <c r="Q177" t="s">
+        <v>500</v>
+      </c>
       <c r="R177" t="s">
         <v>353</v>
       </c>
@@ -10311,6 +10357,15 @@
       <c r="N178" t="s">
         <v>397</v>
       </c>
+      <c r="O178" t="s">
+        <v>499</v>
+      </c>
+      <c r="P178">
+        <v>1</v>
+      </c>
+      <c r="Q178" t="s">
+        <v>500</v>
+      </c>
       <c r="R178" t="s">
         <v>353</v>
       </c>
@@ -10407,6 +10462,15 @@
       <c r="N180" t="s">
         <v>397</v>
       </c>
+      <c r="O180" t="s">
+        <v>499</v>
+      </c>
+      <c r="P180">
+        <v>1</v>
+      </c>
+      <c r="Q180" t="s">
+        <v>500</v>
+      </c>
       <c r="R180" t="s">
         <v>353</v>
       </c>
@@ -10455,6 +10519,15 @@
       <c r="N181" t="s">
         <v>397</v>
       </c>
+      <c r="O181" t="s">
+        <v>499</v>
+      </c>
+      <c r="P181">
+        <v>1</v>
+      </c>
+      <c r="Q181" t="s">
+        <v>500</v>
+      </c>
       <c r="R181" t="s">
         <v>353</v>
       </c>
@@ -10503,6 +10576,15 @@
       <c r="N182" t="s">
         <v>397</v>
       </c>
+      <c r="O182" t="s">
+        <v>499</v>
+      </c>
+      <c r="P182">
+        <v>1</v>
+      </c>
+      <c r="Q182" t="s">
+        <v>500</v>
+      </c>
       <c r="R182" t="s">
         <v>353</v>
       </c>
@@ -10647,6 +10729,15 @@
       <c r="N185" t="s">
         <v>397</v>
       </c>
+      <c r="O185" t="s">
+        <v>499</v>
+      </c>
+      <c r="P185">
+        <v>1</v>
+      </c>
+      <c r="Q185" t="s">
+        <v>500</v>
+      </c>
       <c r="R185" t="s">
         <v>353</v>
       </c>
@@ -10695,6 +10786,15 @@
       <c r="N186" t="s">
         <v>397</v>
       </c>
+      <c r="O186" t="s">
+        <v>499</v>
+      </c>
+      <c r="P186">
+        <v>1</v>
+      </c>
+      <c r="Q186" t="s">
+        <v>500</v>
+      </c>
       <c r="R186" t="s">
         <v>353</v>
       </c>
@@ -10983,6 +11083,15 @@
       <c r="N192" t="s">
         <v>397</v>
       </c>
+      <c r="O192" t="s">
+        <v>499</v>
+      </c>
+      <c r="P192">
+        <v>1</v>
+      </c>
+      <c r="Q192" t="s">
+        <v>500</v>
+      </c>
       <c r="R192" t="s">
         <v>353</v>
       </c>
@@ -11127,6 +11236,15 @@
       <c r="N195" t="s">
         <v>397</v>
       </c>
+      <c r="O195" t="s">
+        <v>499</v>
+      </c>
+      <c r="P195">
+        <v>1</v>
+      </c>
+      <c r="Q195" t="s">
+        <v>500</v>
+      </c>
       <c r="R195" t="s">
         <v>353</v>
       </c>
@@ -11271,6 +11389,15 @@
       <c r="N198" t="s">
         <v>397</v>
       </c>
+      <c r="O198" t="s">
+        <v>499</v>
+      </c>
+      <c r="P198">
+        <v>1</v>
+      </c>
+      <c r="Q198" t="s">
+        <v>500</v>
+      </c>
       <c r="R198" t="s">
         <v>353</v>
       </c>
@@ -11319,6 +11446,15 @@
       <c r="N199" t="s">
         <v>397</v>
       </c>
+      <c r="O199" t="s">
+        <v>499</v>
+      </c>
+      <c r="P199">
+        <v>1</v>
+      </c>
+      <c r="Q199" t="s">
+        <v>500</v>
+      </c>
       <c r="R199" t="s">
         <v>353</v>
       </c>
@@ -11367,6 +11503,15 @@
       <c r="N200" t="s">
         <v>397</v>
       </c>
+      <c r="O200" t="s">
+        <v>499</v>
+      </c>
+      <c r="P200">
+        <v>1</v>
+      </c>
+      <c r="Q200" t="s">
+        <v>500</v>
+      </c>
       <c r="R200" t="s">
         <v>353</v>
       </c>
@@ -17586,6 +17731,12 @@
       <c r="N337" t="s">
         <v>397</v>
       </c>
+      <c r="O337" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q337" t="s">
+        <v>501</v>
+      </c>
       <c r="R337" t="s">
         <v>481</v>
       </c>
@@ -17634,6 +17785,12 @@
       <c r="N338" t="s">
         <v>397</v>
       </c>
+      <c r="O338" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q338" t="s">
+        <v>501</v>
+      </c>
       <c r="R338" t="s">
         <v>481</v>
       </c>
@@ -17682,6 +17839,12 @@
       <c r="N339" t="s">
         <v>397</v>
       </c>
+      <c r="O339" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q339" t="s">
+        <v>501</v>
+      </c>
       <c r="R339" t="s">
         <v>481</v>
       </c>
@@ -17730,6 +17893,12 @@
       <c r="N340" t="s">
         <v>397</v>
       </c>
+      <c r="O340" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q340" t="s">
+        <v>501</v>
+      </c>
       <c r="R340" t="s">
         <v>481</v>
       </c>
@@ -17778,6 +17947,12 @@
       <c r="N341" t="s">
         <v>397</v>
       </c>
+      <c r="O341" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q341" t="s">
+        <v>501</v>
+      </c>
       <c r="R341" t="s">
         <v>481</v>
       </c>
@@ -17874,6 +18049,12 @@
       <c r="N343" t="s">
         <v>397</v>
       </c>
+      <c r="O343" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q343" t="s">
+        <v>501</v>
+      </c>
       <c r="R343" t="s">
         <v>481</v>
       </c>
@@ -17922,6 +18103,12 @@
       <c r="N344" t="s">
         <v>397</v>
       </c>
+      <c r="O344" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q344" t="s">
+        <v>501</v>
+      </c>
       <c r="R344" t="s">
         <v>481</v>
       </c>
@@ -17970,6 +18157,12 @@
       <c r="N345" t="s">
         <v>397</v>
       </c>
+      <c r="O345" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q345" t="s">
+        <v>501</v>
+      </c>
       <c r="R345" t="s">
         <v>481</v>
       </c>
@@ -18018,6 +18211,12 @@
       <c r="N346" t="s">
         <v>397</v>
       </c>
+      <c r="O346" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q346" t="s">
+        <v>501</v>
+      </c>
       <c r="R346" t="s">
         <v>481</v>
       </c>
@@ -18066,6 +18265,12 @@
       <c r="N347" t="s">
         <v>397</v>
       </c>
+      <c r="O347" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q347" t="s">
+        <v>501</v>
+      </c>
       <c r="R347" t="s">
         <v>481</v>
       </c>
@@ -18114,6 +18319,12 @@
       <c r="N348" t="s">
         <v>397</v>
       </c>
+      <c r="O348" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q348" t="s">
+        <v>501</v>
+      </c>
       <c r="R348" t="s">
         <v>481</v>
       </c>
@@ -18162,6 +18373,12 @@
       <c r="N349" t="s">
         <v>397</v>
       </c>
+      <c r="O349" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q349" t="s">
+        <v>501</v>
+      </c>
       <c r="R349" t="s">
         <v>481</v>
       </c>
@@ -18210,6 +18427,12 @@
       <c r="N350" t="s">
         <v>397</v>
       </c>
+      <c r="O350" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q350" t="s">
+        <v>501</v>
+      </c>
       <c r="R350" t="s">
         <v>481</v>
       </c>
@@ -18258,6 +18481,12 @@
       <c r="N351" t="s">
         <v>397</v>
       </c>
+      <c r="O351" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q351" t="s">
+        <v>501</v>
+      </c>
       <c r="R351" t="s">
         <v>481</v>
       </c>
@@ -18306,6 +18535,12 @@
       <c r="N352" t="s">
         <v>397</v>
       </c>
+      <c r="O352" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q352" t="s">
+        <v>501</v>
+      </c>
       <c r="R352" t="s">
         <v>481</v>
       </c>
@@ -18354,6 +18589,12 @@
       <c r="N353" t="s">
         <v>397</v>
       </c>
+      <c r="O353" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q353" t="s">
+        <v>501</v>
+      </c>
       <c r="R353" t="s">
         <v>481</v>
       </c>
@@ -18402,6 +18643,12 @@
       <c r="N354" t="s">
         <v>397</v>
       </c>
+      <c r="O354" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q354" t="s">
+        <v>501</v>
+      </c>
       <c r="R354" t="s">
         <v>481</v>
       </c>
@@ -18450,6 +18697,12 @@
       <c r="N355" t="s">
         <v>397</v>
       </c>
+      <c r="O355" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q355" t="s">
+        <v>501</v>
+      </c>
       <c r="R355" t="s">
         <v>481</v>
       </c>
@@ -18498,6 +18751,12 @@
       <c r="N356" t="s">
         <v>397</v>
       </c>
+      <c r="O356" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q356" t="s">
+        <v>501</v>
+      </c>
       <c r="R356" t="s">
         <v>481</v>
       </c>
@@ -18546,6 +18805,12 @@
       <c r="N357" t="s">
         <v>397</v>
       </c>
+      <c r="O357" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q357" t="s">
+        <v>501</v>
+      </c>
       <c r="R357" t="s">
         <v>481</v>
       </c>
@@ -18594,6 +18859,12 @@
       <c r="N358" t="s">
         <v>397</v>
       </c>
+      <c r="O358" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q358" t="s">
+        <v>501</v>
+      </c>
       <c r="R358" t="s">
         <v>481</v>
       </c>
@@ -18642,6 +18913,12 @@
       <c r="N359" t="s">
         <v>397</v>
       </c>
+      <c r="O359" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q359" t="s">
+        <v>501</v>
+      </c>
       <c r="R359" t="s">
         <v>481</v>
       </c>
@@ -18690,6 +18967,12 @@
       <c r="N360" t="s">
         <v>397</v>
       </c>
+      <c r="O360" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q360" t="s">
+        <v>501</v>
+      </c>
       <c r="R360" t="s">
         <v>481</v>
       </c>
@@ -18738,6 +19021,12 @@
       <c r="N361" t="s">
         <v>397</v>
       </c>
+      <c r="O361" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q361" t="s">
+        <v>501</v>
+      </c>
       <c r="R361" t="s">
         <v>481</v>
       </c>
@@ -18786,6 +19075,12 @@
       <c r="N362" t="s">
         <v>397</v>
       </c>
+      <c r="O362" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q362" t="s">
+        <v>501</v>
+      </c>
       <c r="R362" t="s">
         <v>481</v>
       </c>
@@ -18834,6 +19129,12 @@
       <c r="N363" t="s">
         <v>397</v>
       </c>
+      <c r="O363" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q363" t="s">
+        <v>501</v>
+      </c>
       <c r="R363" t="s">
         <v>481</v>
       </c>
@@ -18882,6 +19183,12 @@
       <c r="N364" t="s">
         <v>397</v>
       </c>
+      <c r="O364" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q364" t="s">
+        <v>501</v>
+      </c>
       <c r="R364" t="s">
         <v>481</v>
       </c>
@@ -18930,6 +19237,12 @@
       <c r="N365" t="s">
         <v>397</v>
       </c>
+      <c r="O365" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q365" t="s">
+        <v>501</v>
+      </c>
       <c r="R365" t="s">
         <v>481</v>
       </c>
@@ -18978,6 +19291,12 @@
       <c r="N366" t="s">
         <v>397</v>
       </c>
+      <c r="O366" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q366" t="s">
+        <v>501</v>
+      </c>
       <c r="R366" t="s">
         <v>481</v>
       </c>
@@ -19026,6 +19345,12 @@
       <c r="N367" t="s">
         <v>397</v>
       </c>
+      <c r="O367" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q367" t="s">
+        <v>501</v>
+      </c>
       <c r="R367" t="s">
         <v>481</v>
       </c>
@@ -19074,6 +19399,12 @@
       <c r="N368" t="s">
         <v>397</v>
       </c>
+      <c r="O368" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q368" t="s">
+        <v>501</v>
+      </c>
       <c r="R368" t="s">
         <v>481</v>
       </c>
@@ -19122,6 +19453,12 @@
       <c r="N369" t="s">
         <v>397</v>
       </c>
+      <c r="O369" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q369" t="s">
+        <v>501</v>
+      </c>
       <c r="R369" t="s">
         <v>481</v>
       </c>
@@ -19170,6 +19507,12 @@
       <c r="N370" t="s">
         <v>397</v>
       </c>
+      <c r="O370" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q370" t="s">
+        <v>501</v>
+      </c>
       <c r="R370" t="s">
         <v>481</v>
       </c>
@@ -19218,6 +19561,12 @@
       <c r="N371" t="s">
         <v>397</v>
       </c>
+      <c r="O371" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q371" t="s">
+        <v>501</v>
+      </c>
       <c r="R371" t="s">
         <v>481</v>
       </c>
@@ -19266,6 +19615,12 @@
       <c r="N372" t="s">
         <v>397</v>
       </c>
+      <c r="O372" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q372" t="s">
+        <v>501</v>
+      </c>
       <c r="R372" t="s">
         <v>481</v>
       </c>
@@ -19314,6 +19669,12 @@
       <c r="N373" t="s">
         <v>397</v>
       </c>
+      <c r="O373" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q373" t="s">
+        <v>501</v>
+      </c>
       <c r="R373" t="s">
         <v>481</v>
       </c>
@@ -19362,6 +19723,12 @@
       <c r="N374" t="s">
         <v>397</v>
       </c>
+      <c r="O374" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q374" t="s">
+        <v>501</v>
+      </c>
       <c r="R374" t="s">
         <v>481</v>
       </c>
@@ -19410,6 +19777,12 @@
       <c r="N375" t="s">
         <v>397</v>
       </c>
+      <c r="O375" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q375" t="s">
+        <v>501</v>
+      </c>
       <c r="R375" t="s">
         <v>481</v>
       </c>
@@ -19458,6 +19831,12 @@
       <c r="N376" t="s">
         <v>397</v>
       </c>
+      <c r="O376" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q376" t="s">
+        <v>501</v>
+      </c>
       <c r="R376" t="s">
         <v>481</v>
       </c>
@@ -19506,6 +19885,12 @@
       <c r="N377" t="s">
         <v>397</v>
       </c>
+      <c r="O377" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q377" t="s">
+        <v>501</v>
+      </c>
       <c r="R377" t="s">
         <v>481</v>
       </c>
@@ -19554,6 +19939,12 @@
       <c r="N378" t="s">
         <v>397</v>
       </c>
+      <c r="O378" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q378" t="s">
+        <v>501</v>
+      </c>
       <c r="R378" t="s">
         <v>481</v>
       </c>
@@ -19602,6 +19993,12 @@
       <c r="N379" t="s">
         <v>397</v>
       </c>
+      <c r="O379" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q379" t="s">
+        <v>501</v>
+      </c>
       <c r="R379" t="s">
         <v>481</v>
       </c>
@@ -19650,6 +20047,12 @@
       <c r="N380" t="s">
         <v>397</v>
       </c>
+      <c r="O380" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q380" t="s">
+        <v>501</v>
+      </c>
       <c r="R380" t="s">
         <v>481</v>
       </c>
@@ -19698,6 +20101,12 @@
       <c r="N381" t="s">
         <v>397</v>
       </c>
+      <c r="O381" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q381" t="s">
+        <v>501</v>
+      </c>
       <c r="R381" t="s">
         <v>481</v>
       </c>
@@ -19794,6 +20203,12 @@
       <c r="N383" t="s">
         <v>397</v>
       </c>
+      <c r="O383" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q383" t="s">
+        <v>501</v>
+      </c>
       <c r="R383" t="s">
         <v>481</v>
       </c>
@@ -19842,6 +20257,12 @@
       <c r="N384" t="s">
         <v>397</v>
       </c>
+      <c r="O384" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q384" t="s">
+        <v>501</v>
+      </c>
       <c r="R384" t="s">
         <v>481</v>
       </c>
@@ -19890,6 +20311,12 @@
       <c r="N385" t="s">
         <v>397</v>
       </c>
+      <c r="O385" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q385" t="s">
+        <v>501</v>
+      </c>
       <c r="R385" t="s">
         <v>481</v>
       </c>
@@ -19938,6 +20365,12 @@
       <c r="N386" t="s">
         <v>397</v>
       </c>
+      <c r="O386" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q386" t="s">
+        <v>501</v>
+      </c>
       <c r="R386" t="s">
         <v>481</v>
       </c>
@@ -19986,6 +20419,12 @@
       <c r="N387" t="s">
         <v>397</v>
       </c>
+      <c r="O387" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q387" t="s">
+        <v>501</v>
+      </c>
       <c r="R387" t="s">
         <v>481</v>
       </c>
@@ -20034,6 +20473,12 @@
       <c r="N388" t="s">
         <v>397</v>
       </c>
+      <c r="O388" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q388" t="s">
+        <v>501</v>
+      </c>
       <c r="R388" t="s">
         <v>481</v>
       </c>
@@ -20082,6 +20527,12 @@
       <c r="N389" t="s">
         <v>397</v>
       </c>
+      <c r="O389" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q389" t="s">
+        <v>501</v>
+      </c>
       <c r="R389" t="s">
         <v>481</v>
       </c>
@@ -20130,6 +20581,12 @@
       <c r="N390" t="s">
         <v>397</v>
       </c>
+      <c r="O390" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q390" t="s">
+        <v>501</v>
+      </c>
       <c r="R390" t="s">
         <v>481</v>
       </c>
@@ -20178,6 +20635,12 @@
       <c r="N391" t="s">
         <v>397</v>
       </c>
+      <c r="O391" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q391" t="s">
+        <v>501</v>
+      </c>
       <c r="R391" t="s">
         <v>481</v>
       </c>
@@ -20226,6 +20689,12 @@
       <c r="N392" t="s">
         <v>397</v>
       </c>
+      <c r="O392" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q392" t="s">
+        <v>501</v>
+      </c>
       <c r="R392" t="s">
         <v>481</v>
       </c>
@@ -20274,6 +20743,12 @@
       <c r="N393" t="s">
         <v>397</v>
       </c>
+      <c r="O393" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q393" t="s">
+        <v>501</v>
+      </c>
       <c r="R393" t="s">
         <v>481</v>
       </c>
@@ -20322,6 +20797,12 @@
       <c r="N394" t="s">
         <v>397</v>
       </c>
+      <c r="O394" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q394" t="s">
+        <v>501</v>
+      </c>
       <c r="R394" t="s">
         <v>481</v>
       </c>
@@ -20370,6 +20851,12 @@
       <c r="N395" t="s">
         <v>397</v>
       </c>
+      <c r="O395" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q395" t="s">
+        <v>501</v>
+      </c>
       <c r="R395" t="s">
         <v>481</v>
       </c>
@@ -20418,6 +20905,12 @@
       <c r="N396" t="s">
         <v>397</v>
       </c>
+      <c r="O396" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q396" t="s">
+        <v>501</v>
+      </c>
       <c r="R396" t="s">
         <v>481</v>
       </c>
@@ -20466,6 +20959,12 @@
       <c r="N397" t="s">
         <v>397</v>
       </c>
+      <c r="O397" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q397" t="s">
+        <v>501</v>
+      </c>
       <c r="R397" t="s">
         <v>481</v>
       </c>
@@ -20514,6 +21013,12 @@
       <c r="N398" t="s">
         <v>397</v>
       </c>
+      <c r="O398" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q398" t="s">
+        <v>501</v>
+      </c>
       <c r="R398" t="s">
         <v>481</v>
       </c>
@@ -20562,6 +21067,12 @@
       <c r="N399" t="s">
         <v>397</v>
       </c>
+      <c r="O399" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q399" t="s">
+        <v>501</v>
+      </c>
       <c r="R399" t="s">
         <v>481</v>
       </c>
@@ -20610,6 +21121,12 @@
       <c r="N400" t="s">
         <v>397</v>
       </c>
+      <c r="O400" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q400" t="s">
+        <v>501</v>
+      </c>
       <c r="R400" t="s">
         <v>481</v>
       </c>
@@ -20658,6 +21175,12 @@
       <c r="N401" t="s">
         <v>397</v>
       </c>
+      <c r="O401" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q401" t="s">
+        <v>501</v>
+      </c>
       <c r="R401" t="s">
         <v>481</v>
       </c>
@@ -20705,6 +21228,12 @@
       </c>
       <c r="N402" t="s">
         <v>397</v>
+      </c>
+      <c r="O402" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q402" t="s">
+        <v>501</v>
       </c>
       <c r="R402" t="s">
         <v>481</v>

</xml_diff>

<commit_message>
edit and create rmd
</commit_message>
<xml_diff>
--- a/data/master-qubit.xlsx
+++ b/data/master-qubit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3D0DDB-CAFF-084C-8F61-0BEC7AA2FAAC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827CF1F6-0AB5-5B4F-BA14-FDD1B6232833}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25560" windowHeight="14900" xr2:uid="{C961D9B2-DEF5-3E45-BFAA-11F0CD1F34D4}"/>
+    <workbookView xWindow="7100" yWindow="560" windowWidth="25560" windowHeight="14900" xr2:uid="{C961D9B2-DEF5-3E45-BFAA-11F0CD1F34D4}"/>
   </bookViews>
   <sheets>
     <sheet name="qubit-iso" sheetId="1" r:id="rId1"/>
@@ -1931,8 +1931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EE0E31-7CFF-2843-B4D6-D974DF19D232}">
   <dimension ref="A1:U402"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P165" sqref="P165"/>
+    <sheetView tabSelected="1" topLeftCell="F228" workbookViewId="0">
+      <selection activeCell="L236" sqref="L236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -13148,11 +13148,11 @@
         <v>332</v>
       </c>
       <c r="L234">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M234">
         <f>(F234)*(L234-G234)</f>
-        <v>371.8</v>
+        <v>314.60000000000002</v>
       </c>
       <c r="N234" t="s">
         <v>397</v>
@@ -13196,11 +13196,11 @@
         <v>332</v>
       </c>
       <c r="L235">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M235">
         <f t="shared" ref="M235:M254" si="9">(F235)*(L235-G235)</f>
-        <v>325</v>
+        <v>275</v>
       </c>
       <c r="N235" t="s">
         <v>397</v>

</xml_diff>